<commit_message>
Excel verbessert, Rendite Risiko angepasst, Sonstiges
</commit_message>
<xml_diff>
--- a/Files/DatenUebersichtC.xlsx
+++ b/Files/DatenUebersichtC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\Desktop 3\AQM MÄRZ 2018\DB Designer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\Desktop 3\eclipse\Repos\PortfolioBro\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0CF1BE-A205-4A3D-96C3-FD936EF3479A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE5C5D2-ACC3-42EE-A795-D5783F9ECDD8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="0" windowWidth="22296" windowHeight="7704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="22296" windowHeight="7704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -60,18 +60,12 @@
     <t>Silber</t>
   </si>
   <si>
-    <t>Energie</t>
-  </si>
-  <si>
     <t>Industriemetalle</t>
   </si>
   <si>
     <t>Benzin</t>
   </si>
   <si>
-    <t>Diesel</t>
-  </si>
-  <si>
     <t>Erdgas</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>Zink</t>
+  </si>
+  <si>
+    <t>Energie u. weiteres</t>
+  </si>
+  <si>
+    <t>Kakao</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,10 +531,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -545,35 +545,35 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>3015</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>2773</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -582,35 +582,35 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>3480</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10">
-        <v>3054</v>
+        <v>2943</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11">
-        <v>2943</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -618,7 +618,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
System.out.println, ImportGUI, Excel Dateien
</commit_message>
<xml_diff>
--- a/Files/DatenUebersichtC.xlsx
+++ b/Files/DatenUebersichtC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\Desktop 3\eclipse\Repos\PortfolioBro\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nilsk\Desktop 3\Swing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE5C5D2-ACC3-42EE-A795-D5783F9ECDD8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAD6190-2A4E-451D-BCF5-0C456F7C5960}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="22296" windowHeight="7704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7812" yWindow="0" windowWidth="22296" windowHeight="7704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>Handelsplatz</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Industriemetalle</t>
   </si>
   <si>
-    <t>Benzin</t>
-  </si>
-  <si>
     <t>Erdgas</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>Kakao</t>
+  </si>
+  <si>
+    <t>Holz</t>
+  </si>
+  <si>
+    <t>Rind</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,13 +537,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>3064</v>
+        <v>2773</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -548,13 +551,13 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>2773</v>
+        <v>3480</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -562,13 +565,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>3480</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -582,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="E9">
-        <v>3054</v>
+        <v>2943</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -596,15 +599,15 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>2943</v>
+        <v>3053</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -618,12 +621,26 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
         <v>3053</v>
       </c>
     </row>

</xml_diff>